<commit_message>
Adjusted files in y2025_2026
</commit_message>
<xml_diff>
--- a/y2025_2026/variables.xlsx
+++ b/y2025_2026/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Barrett\Documents\#Uni\ME3\DMT Temp\Code\ME3-DMT-5\y2025_2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EF221F-2074-44B6-9AE2-A6A6B65D517E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A685663D-772C-448A-A265-75153B24463B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{40717EA2-1D2E-4F0B-89AE-8B7A7849C616}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pe</t>
   </si>
@@ -60,13 +60,34 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>emissivity</t>
+  </si>
+  <si>
+    <t>rc</t>
+  </si>
+  <si>
+    <t>mu_0</t>
+  </si>
+  <si>
+    <t>Cp_0</t>
+  </si>
+  <si>
+    <t>Pr_0</t>
+  </si>
+  <si>
+    <t>wall_thick</t>
+  </si>
+  <si>
+    <t>inregen_wall_thick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +98,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE06C75"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -101,9 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -440,13 +470,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAD4DDD-7E4D-4ABF-9720-B8AE4BD5F236}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -512,6 +546,67 @@
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.06</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6.8480000000000008E-5</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1.9</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.57579999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>